<commit_message>
Adaptation for greenhouse project
</commit_message>
<xml_diff>
--- a/PhD-MRS-Optimization-EA/coefs.xlsx
+++ b/PhD-MRS-Optimization-EA/coefs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>X</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>f2</t>
+  </si>
+  <si>
+    <t>mult</t>
   </si>
 </sst>
 </file>
@@ -172,54 +175,39 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$B$22</c:f>
+              <c:f>Sheet1!$B$8:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>1.3888888888888889E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>1.3888888888888889E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>1.3888888888888889E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>1.3888888888888889E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>1.3888888888888889E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>1.3888888888888889E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>1.3888888888888889E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>1.3888888888888889E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>1.3888888888888889E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>10</c:v>
+                  <c:v>1.3888888888888889E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -248,54 +236,39 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$22</c:f>
+              <c:f>Sheet1!$C$8:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>1.3888888888888889E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>2.7777777777777778E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>4.1666666666666664E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>5.5555555555555556E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>6.9444444444444447E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>8.3333333333333328E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35</c:v>
+                  <c:v>9.7222222222222219E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40</c:v>
+                  <c:v>1.1111111111111111E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45</c:v>
+                  <c:v>1.25E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>75</c:v>
+                  <c:v>1.3888888888888889E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -324,54 +297,39 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$8:$D$22</c:f>
+              <c:f>Sheet1!$D$8:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.02</c:v>
+                  <c:v>2.7777777777777779E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16</c:v>
+                  <c:v>1.1111111111111112E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.54</c:v>
+                  <c:v>2.5000000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.28</c:v>
+                  <c:v>4.4444444444444447E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5</c:v>
+                  <c:v>6.9444444444444447E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.32</c:v>
+                  <c:v>1E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.86</c:v>
+                  <c:v>1.3611111111111111E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.24</c:v>
+                  <c:v>1.7777777777777779E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14.58</c:v>
+                  <c:v>2.2500000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>26.62</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>34.56</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>43.94</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>54.88</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>67.5</c:v>
+                  <c:v>2.7777777777777779E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -400,54 +358,39 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$8:$E$22</c:f>
+              <c:f>Sheet1!$E$8:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>15.02</c:v>
+                  <c:v>1.5555555555555557E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.16</c:v>
+                  <c:v>1.7777777777777779E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.54</c:v>
+                  <c:v>2.0555555555555553E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31.28</c:v>
+                  <c:v>2.3888888888888887E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.5</c:v>
+                  <c:v>2.7777777777777779E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44.32</c:v>
+                  <c:v>3.2222222222222222E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>51.86</c:v>
+                  <c:v>3.7222222222222223E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60.24</c:v>
+                  <c:v>4.2777777777777779E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>69.58</c:v>
+                  <c:v>4.8888888888888888E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>91.62</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>104.56</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>118.94</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>134.88</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>152.5</c:v>
+                  <c:v>5.5555555555555558E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -462,11 +405,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="48391296"/>
-        <c:axId val="144990208"/>
+        <c:axId val="98001664"/>
+        <c:axId val="98003200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48391296"/>
+        <c:axId val="98001664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -475,13 +418,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144990208"/>
+        <c:crossAx val="98003200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="144990208"/>
+        <c:axId val="98003200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -492,7 +435,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48391296"/>
+        <c:crossAx val="98001664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1433,11 +1376,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="152916736"/>
-        <c:axId val="152918272"/>
+        <c:axId val="98307072"/>
+        <c:axId val="98317056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="152916736"/>
+        <c:axId val="98307072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1447,7 +1390,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152918272"/>
+        <c:crossAx val="98317056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1455,7 +1398,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152918272"/>
+        <c:axId val="98317056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -1467,7 +1410,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152916736"/>
+        <c:crossAx val="98307072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1831,11 +1774,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="88016768"/>
-        <c:axId val="88015232"/>
+        <c:axId val="133379584"/>
+        <c:axId val="133381120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88016768"/>
+        <c:axId val="133379584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -1846,12 +1789,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88015232"/>
+        <c:crossAx val="133381120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88015232"/>
+        <c:axId val="133381120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1862,7 +1805,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88016768"/>
+        <c:crossAx val="133379584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2276,19 +2219,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -2302,21 +2246,43 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>10</v>
+        <f>B3/$B$5</f>
+        <v>1.3888888888888889E-3</v>
       </c>
       <c r="C2">
+        <f>C3/$B$5</f>
+        <v>1.3888888888888889E-4</v>
+      </c>
+      <c r="D2">
+        <f>D3/$B$5</f>
+        <v>2.7777777777777779E-5</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3">
         <v>5</v>
       </c>
-      <c r="D2">
-        <v>0.02</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -2333,324 +2299,290 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" s="2">
         <f>$B$2</f>
-        <v>10</v>
+        <v>1.3888888888888889E-3</v>
       </c>
       <c r="C8" s="2">
         <f>$C$2*A8</f>
-        <v>5</v>
+        <v>1.3888888888888889E-4</v>
       </c>
       <c r="D8" s="2">
         <f>$D$2*A8^$E$2</f>
-        <v>0.02</v>
+        <v>2.7777777777777779E-5</v>
       </c>
       <c r="E8" s="2">
         <f>SUM(B8:D8)</f>
-        <v>15.02</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.5555555555555557E-3</v>
+      </c>
+      <c r="F8">
+        <f>E8*$B$5</f>
+        <v>5.6000000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" ref="B9:B22" si="0">$B$2</f>
-        <v>10</v>
+        <v>1.3888888888888889E-3</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" ref="C9:C22" si="1">$C$2*A9</f>
-        <v>10</v>
+        <v>2.7777777777777778E-4</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" ref="D9:D22" si="2">$D$2*A9^$E$2</f>
-        <v>0.16</v>
+        <v>1.1111111111111112E-4</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" ref="E9:E22" si="3">SUM(B9:D9)</f>
-        <v>20.16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.7777777777777779E-3</v>
+      </c>
+      <c r="F9">
+        <f>E9*$B$5</f>
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1.3888888888888889E-3</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>4.1666666666666664E-4</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="2"/>
-        <v>0.54</v>
+        <v>2.5000000000000001E-4</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="3"/>
-        <v>25.54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2.0555555555555553E-3</v>
+      </c>
+      <c r="F10">
+        <f>E10*$B$5</f>
+        <v>7.3999999999999986</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1.3888888888888889E-3</v>
       </c>
       <c r="C11" s="2">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>5.5555555555555556E-4</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="2"/>
-        <v>1.28</v>
+        <v>4.4444444444444447E-4</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="3"/>
-        <v>31.28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2.3888888888888887E-3</v>
+      </c>
+      <c r="F11">
+        <f>E11*$B$5</f>
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1.3888888888888889E-3</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>6.9444444444444447E-4</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>6.9444444444444447E-4</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" si="3"/>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="F12">
+        <f>E12*$B$5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1.3888888888888889E-3</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>8.3333333333333328E-4</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="2"/>
-        <v>4.32</v>
+        <v>1E-3</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="3"/>
-        <v>44.32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3.2222222222222222E-3</v>
+      </c>
+      <c r="F13">
+        <f>E13*$B$5</f>
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1.3888888888888889E-3</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>9.7222222222222219E-4</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="2"/>
-        <v>6.86</v>
+        <v>1.3611111111111111E-3</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="3"/>
-        <v>51.86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3.7222222222222223E-3</v>
+      </c>
+      <c r="F14">
+        <f>E14*$B$5</f>
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>8</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1.3888888888888889E-3</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>1.1111111111111111E-3</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="2"/>
-        <v>10.24</v>
+        <v>1.7777777777777779E-3</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="3"/>
-        <v>60.24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.2777777777777779E-3</v>
+      </c>
+      <c r="F15">
+        <f>E15*$B$5</f>
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1.3888888888888889E-3</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>1.25E-3</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="2"/>
-        <v>14.58</v>
+        <v>2.2500000000000003E-3</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="3"/>
-        <v>69.58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4.8888888888888888E-3</v>
+      </c>
+      <c r="F16">
+        <f>E16*$B$5</f>
+        <v>17.600000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1.3888888888888889E-3</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>1.3888888888888889E-3</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>2.7777777777777779E-3</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="3"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>11</v>
-      </c>
-      <c r="B18" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C18" s="2">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="D18" s="2">
-        <f t="shared" si="2"/>
-        <v>26.62</v>
-      </c>
-      <c r="E18" s="2">
-        <f t="shared" si="3"/>
-        <v>91.62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>12</v>
-      </c>
-      <c r="B19" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C19" s="2">
-        <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="D19" s="2">
-        <f t="shared" si="2"/>
-        <v>34.56</v>
-      </c>
-      <c r="E19" s="2">
-        <f t="shared" si="3"/>
-        <v>104.56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>13</v>
-      </c>
-      <c r="B20" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C20" s="2">
-        <f t="shared" si="1"/>
-        <v>65</v>
-      </c>
-      <c r="D20" s="2">
-        <f t="shared" si="2"/>
-        <v>43.94</v>
-      </c>
-      <c r="E20" s="2">
-        <f t="shared" si="3"/>
-        <v>118.94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>14</v>
-      </c>
-      <c r="B21" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C21" s="2">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="D21" s="2">
-        <f t="shared" si="2"/>
-        <v>54.88</v>
-      </c>
-      <c r="E21" s="2">
-        <f t="shared" si="3"/>
-        <v>134.88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>15</v>
-      </c>
-      <c r="B22" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C22" s="2">
-        <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
-      <c r="D22" s="2">
-        <f t="shared" si="2"/>
-        <v>67.5</v>
-      </c>
-      <c r="E22" s="2">
-        <f t="shared" si="3"/>
-        <v>152.5</v>
-      </c>
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="F17">
+        <f>E17*$B$5</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3275,9 +3207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>